<commit_message>
mise en page des tableaux
</commit_message>
<xml_diff>
--- a/Excel_Exercice01_MiseEnFormeEtGraphique.xlsx
+++ b/Excel_Exercice01_MiseEnFormeEtGraphique.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="123820"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\repo lab OG\C13---Outils-de-gestion-et-de-soutien\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B31C70C-7A1D-4CD0-858F-BBBAAD6FB1E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3D73E7-F597-4BC8-83EC-8D8876C4AB5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -134,9 +134,6 @@
     <t>Courbes avec marques</t>
   </si>
   <si>
-    <t>Étiquettes de lignes</t>
-  </si>
-  <si>
     <t>Total général</t>
   </si>
   <si>
@@ -154,6 +151,9 @@
   <si>
     <t>Somme de Total</t>
   </si>
+  <si>
+    <t>ventes</t>
+  </si>
 </sst>
 </file>
 
@@ -164,7 +164,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;$&quot;"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,8 +316,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -378,8 +385,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="34">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -786,13 +817,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1010,10 +1074,6 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
@@ -1039,13 +1099,267 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Milliers" xfId="1" builtinId="3"/>
     <cellStyle name="Monétaire" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="38">
+    <dxf>
+      <border>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1053,10 +1367,49 @@
         <color rgb="FF9C0006"/>
       </font>
     </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCC0000"/>
       <color rgb="FFECF2F8"/>
       <color rgb="FFEBE3E3"/>
     </mruColors>
@@ -5573,15 +5926,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1031875</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>536575</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5826,8 +6179,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BDEC5865-4DA1-4D5C-A852-85F7BAC32AD9}" name="Tableau croisé dynamique3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B17:G19" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BDEC5865-4DA1-4D5C-A852-85F7BAC32AD9}" name="Tableau croisé dynamique3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Net">
+  <location ref="B19:G21" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0">
       <items count="2">
@@ -5879,6 +6232,86 @@
     <dataField name="Somme de Trimestre 4" fld="4" baseField="0" baseItem="0"/>
     <dataField name="Somme de Total" fld="5" baseField="0" baseItem="0"/>
   </dataFields>
+  <formats count="12">
+    <format dxfId="21">
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="20">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="5">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="14">
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="13">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="5">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="12">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="11">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="10">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="4">
+      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="3">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="2">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="0">
+      <pivotArea field="0" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -5892,8 +6325,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{79789EE9-0E26-4CF9-A033-86CAC670344D}" name="Tableau croisé dynamique2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B11:G16" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{79789EE9-0E26-4CF9-A033-86CAC670344D}" name="Tableau croisé dynamique2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Dépenses">
+  <location ref="B12:G17" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0">
       <items count="5">
@@ -5957,6 +6390,86 @@
     <dataField name="Somme de Trimestre 4" fld="4" baseField="0" baseItem="0"/>
     <dataField name="Somme de Total" fld="5" baseField="0" baseItem="0"/>
   </dataFields>
+  <formats count="12">
+    <format dxfId="27">
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="26">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="5">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="23">
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="22">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="5">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="17">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="16">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="15">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="9">
+      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="8">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="7">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
+      <pivotArea field="0" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -5970,7 +6483,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{46800AEB-89AF-4544-942D-4BC6AC1EEAA7}" name="Tableau croisé dynamique1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{46800AEB-89AF-4544-942D-4BC6AC1EEAA7}" name="Tableau croisé dynamique1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9" rowHeaderCaption="ventes">
   <location ref="B3:G10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0">
@@ -6043,6 +6556,103 @@
     <dataField name="Somme de Trimestre 4" fld="4" baseField="0" baseItem="0"/>
     <dataField name="Somme de Total" fld="5" baseField="0" baseItem="0"/>
   </dataFields>
+  <formats count="13">
+    <format dxfId="37">
+      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="36">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="35">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="34">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="33">
+      <pivotArea field="0" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="31">
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="30">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="5">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="29">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="28">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="25">
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="24">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="5">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="19">
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="18">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="5">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
   <chartFormats count="30">
     <chartFormat chart="1" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
@@ -6665,24 +7275,24 @@
   <sheetData>
     <row r="1" spans="2:17" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:17" ht="20" x14ac:dyDescent="0.4">
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="60"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58"/>
     </row>
     <row r="3" spans="2:17" ht="3.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="6"/>
@@ -6693,24 +7303,24 @@
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61"/>
-      <c r="M4" s="61"/>
-      <c r="N4" s="61"/>
-      <c r="O4" s="61"/>
-      <c r="P4" s="61"/>
-      <c r="Q4" s="61"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59"/>
+      <c r="Q4" s="59"/>
     </row>
     <row r="5" spans="2:17" ht="3.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6"/>
@@ -7078,7 +7688,7 @@
     <mergeCell ref="B4:Q4"/>
   </mergeCells>
   <conditionalFormatting sqref="C25:G25">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="32" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7107,14 +7717,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" ht="22" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -7466,15 +8076,15 @@
   <sheetData>
     <row r="1" spans="2:4" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
     </row>
     <row r="3" spans="2:4" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="61" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="53" t="s">
@@ -7482,25 +8092,25 @@
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="63"/>
+      <c r="C5" s="61"/>
       <c r="D5" s="54" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="63"/>
+      <c r="C6" s="61"/>
       <c r="D6" s="55" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="63"/>
+      <c r="C7" s="61"/>
       <c r="D7" s="54" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="63"/>
+      <c r="C8" s="61"/>
       <c r="D8" s="56" t="s">
         <v>27</v>
       </c>
@@ -7509,7 +8119,7 @@
       <c r="C9" s="52"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="63" t="s">
+      <c r="C10" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="53" t="s">
@@ -7517,19 +8127,19 @@
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="63"/>
+      <c r="C11" s="61"/>
       <c r="D11" s="54" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="63"/>
+      <c r="C12" s="61"/>
       <c r="D12" s="55" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="63"/>
+      <c r="C13" s="61"/>
       <c r="D13" s="57" t="s">
         <v>23</v>
       </c>
@@ -7548,10 +8158,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33DC3222-9268-4458-8BD2-A01EEBC24E49}">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7563,384 +8173,384 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="26" x14ac:dyDescent="0.6">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="64"/>
+      <c r="Q2" s="64"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B3" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="72" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="72" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" s="73" t="s">
         <v>35</v>
-      </c>
-      <c r="G3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="69">
         <v>2337.81</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="69">
         <v>2137.81</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="69">
         <v>1237.81</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="69">
         <v>3237.81</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="70">
         <v>8951.24</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="69">
         <v>5215</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="69">
         <v>8309.0499999999993</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="69">
         <v>4287.9799999999996</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="69">
         <v>9352.64</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="70">
         <v>27164.67</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="69">
         <v>4336.37</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="69">
         <v>1790.84</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="69">
         <v>1206.77</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="69">
         <v>1628.13</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="70">
         <v>8962.11</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="69">
         <v>1988.5</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="69">
         <v>2897.35</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="69">
         <v>5223.25</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="69">
         <v>7996.36</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="70">
         <v>18105.46</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="69">
         <v>7832.97</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="69">
         <v>11299.87</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="69">
         <v>8264.81</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="69">
         <v>13226.47</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="70">
         <v>40624.120000000003</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="69">
         <v>21710.65</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="69">
         <v>26434.920000000002</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="69">
         <v>20220.620000000003</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="69">
         <v>35441.409999999996</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="70">
         <v>103807.6</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B10" s="59" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="66">
         <v>43421.3</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="66">
         <v>52869.84</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="66">
         <v>40441.240000000005</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="66">
         <v>70882.819999999992</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="67">
         <v>207615.2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B11" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B12" s="59" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12">
-        <v>2533.2399999999998</v>
-      </c>
-      <c r="D12">
-        <v>5855.47</v>
-      </c>
-      <c r="E12">
-        <v>8525.14</v>
-      </c>
-      <c r="F12">
-        <v>11253.21</v>
-      </c>
-      <c r="G12">
-        <v>28167.059999999998</v>
+      <c r="B12" s="71" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="71" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="71" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="71" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="71" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="81" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B13" s="59" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13">
-        <v>12462.87</v>
-      </c>
-      <c r="D13">
-        <v>8256.9699999999993</v>
-      </c>
-      <c r="E13">
-        <v>10884.65</v>
-      </c>
-      <c r="F13">
-        <v>18995.599999999999</v>
-      </c>
-      <c r="G13">
-        <v>50600.09</v>
+      <c r="B13" s="74" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="75">
+        <v>2533.2399999999998</v>
+      </c>
+      <c r="D13" s="75">
+        <v>5855.47</v>
+      </c>
+      <c r="E13" s="75">
+        <v>8525.14</v>
+      </c>
+      <c r="F13" s="75">
+        <v>11253.21</v>
+      </c>
+      <c r="G13" s="82">
+        <v>28167.059999999998</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B14" s="59" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>23751.35</v>
-      </c>
-      <c r="D14">
-        <v>21674.66</v>
-      </c>
-      <c r="E14">
-        <v>24631.350000000002</v>
-      </c>
-      <c r="F14">
-        <v>33505.279999999999</v>
-      </c>
-      <c r="G14">
-        <v>103562.64</v>
+      <c r="B14" s="74" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="75">
+        <v>12462.87</v>
+      </c>
+      <c r="D14" s="75">
+        <v>8256.9699999999993</v>
+      </c>
+      <c r="E14" s="75">
+        <v>10884.65</v>
+      </c>
+      <c r="F14" s="75">
+        <v>18995.599999999999</v>
+      </c>
+      <c r="G14" s="82">
+        <v>50600.09</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B15" s="59" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15">
-        <v>8755.24</v>
-      </c>
-      <c r="D15">
-        <v>7562.22</v>
-      </c>
-      <c r="E15">
-        <v>5221.5600000000004</v>
-      </c>
-      <c r="F15">
-        <v>3256.47</v>
-      </c>
-      <c r="G15">
-        <v>24795.49</v>
+      <c r="B15" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="75">
+        <v>23751.35</v>
+      </c>
+      <c r="D15" s="75">
+        <v>21674.66</v>
+      </c>
+      <c r="E15" s="75">
+        <v>24631.350000000002</v>
+      </c>
+      <c r="F15" s="75">
+        <v>33505.279999999999</v>
+      </c>
+      <c r="G15" s="82">
+        <v>103562.64</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B16" s="59" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16">
-        <v>47502.7</v>
-      </c>
-      <c r="D16">
-        <v>43349.32</v>
-      </c>
-      <c r="E16">
-        <v>49262.7</v>
-      </c>
-      <c r="F16">
-        <v>67010.559999999998</v>
-      </c>
-      <c r="G16">
-        <v>207125.27999999997</v>
+      <c r="B16" s="74" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="75">
+        <v>8755.24</v>
+      </c>
+      <c r="D16" s="75">
+        <v>7562.22</v>
+      </c>
+      <c r="E16" s="75">
+        <v>5221.5600000000004</v>
+      </c>
+      <c r="F16" s="75">
+        <v>3256.47</v>
+      </c>
+      <c r="G16" s="82">
+        <v>24795.49</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="C17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B18" s="59" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>-2040.6999999999971</v>
-      </c>
-      <c r="D18">
-        <v>4760.260000000002</v>
-      </c>
-      <c r="E18">
-        <v>-4410.7299999999996</v>
-      </c>
-      <c r="F18">
-        <v>1936.1299999999974</v>
-      </c>
-      <c r="G18">
-        <v>244.96</v>
+      <c r="C17" s="80">
+        <v>47502.7</v>
+      </c>
+      <c r="D17" s="80">
+        <v>43349.32</v>
+      </c>
+      <c r="E17" s="80">
+        <v>49262.7</v>
+      </c>
+      <c r="F17" s="80">
+        <v>67010.559999999998</v>
+      </c>
+      <c r="G17" s="83">
+        <v>207125.27999999997</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B19" s="59" t="s">
+      <c r="B19" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="C19">
+      <c r="D19" s="76" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="76" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="86" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B20" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="78">
         <v>-2040.6999999999971</v>
       </c>
-      <c r="D19">
+      <c r="D20" s="78">
         <v>4760.260000000002</v>
       </c>
-      <c r="E19">
+      <c r="E20" s="78">
         <v>-4410.7299999999996</v>
       </c>
-      <c r="F19">
+      <c r="F20" s="78">
         <v>1936.1299999999974</v>
       </c>
-      <c r="G19">
+      <c r="G20" s="87">
+        <v>244.96</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B21" s="84" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="85">
+        <v>-2040.6999999999971</v>
+      </c>
+      <c r="D21" s="85">
+        <v>4760.260000000002</v>
+      </c>
+      <c r="E21" s="85">
+        <v>-4410.7299999999996</v>
+      </c>
+      <c r="F21" s="85">
+        <v>1936.1299999999974</v>
+      </c>
+      <c r="G21" s="88">
         <v>244.96</v>
       </c>
     </row>

</xml_diff>